<commit_message>
update CSP violations report
</commit_message>
<xml_diff>
--- a/docs/CSP_violations_clinsight.xlsx
+++ b/docs/CSP_violations_clinsight.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lsamson\Projects\99_data_science\test_server\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20F3E91E-4EEF-4446-8988-7DC9F06474E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18713AB0-0E28-45F1-B560-4DC4B3AD3B12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{FE7073C4-89C7-45DD-9368-D1EB06517403}"/>
+    <workbookView xWindow="28680" yWindow="-6720" windowWidth="29040" windowHeight="15720" xr2:uid="{FE7073C4-89C7-45DD-9368-D1EB06517403}"/>
   </bookViews>
   <sheets>
     <sheet name="hashes" sheetId="1" r:id="rId1"/>
@@ -636,18 +636,18 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="68.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="67.28515625" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="68.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="67.26953125" customWidth="1"/>
+    <col min="4" max="4" width="10.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -661,7 +661,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
@@ -669,7 +669,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -677,7 +677,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>3</v>
       </c>
@@ -685,7 +685,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>41</v>
       </c>
@@ -696,7 +696,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>4</v>
       </c>
@@ -707,7 +707,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -721,7 +721,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -735,7 +735,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -749,7 +749,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -763,7 +763,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -777,7 +777,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -791,7 +791,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -805,7 +805,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -819,7 +819,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>10</v>
       </c>
@@ -833,7 +833,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>10</v>
       </c>
@@ -847,7 +847,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>10</v>
       </c>
@@ -861,7 +861,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>10</v>
       </c>
@@ -875,7 +875,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>10</v>
       </c>
@@ -889,7 +889,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>10</v>
       </c>
@@ -903,7 +903,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>10</v>
       </c>
@@ -917,7 +917,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>10</v>
       </c>
@@ -931,7 +931,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>10</v>
       </c>
@@ -959,13 +959,13 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="180.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="180.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -976,7 +976,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>29</v>
       </c>
@@ -990,7 +990,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -1004,7 +1004,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="120" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="116" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>33</v>
       </c>
@@ -1018,7 +1018,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="300" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="290" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>34</v>
       </c>

</xml_diff>